<commit_message>
updated raw data files
</commit_message>
<xml_diff>
--- a/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
+++ b/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TamiAlade/Desktop/Research/speed-acc/data/0a_demographics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Experiments/KM_SPEED_ACC/bing_data/speed_acc_child_gaze/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3700" yWindow="1320" windowWidth="25100" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="6120" yWindow="1320" windowWidth="25100" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
   <si>
     <t>subid</t>
   </si>
@@ -218,10 +221,10 @@
     <t xml:space="preserve">ended session halfway through the first blcok </t>
   </si>
   <si>
-    <t xml:space="preserve">left the session halfway through </t>
-  </si>
-  <si>
-    <t xml:space="preserve">had thick glasses, could not calibrate </t>
+    <t>first block went well, but child decided to stop early during block 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">played with headphones during a couple of trials, and stood up for a couple of trials, but majority of session went well </t>
   </si>
 </sst>
 </file>
@@ -764,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1240,7 +1243,7 @@
         <v>11</v>
       </c>
       <c r="H23" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1307,103 +1310,203 @@
       <c r="A27" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="B27" s="1">
+        <v>42942</v>
+      </c>
+      <c r="C27" s="1">
+        <v>41153</v>
+      </c>
+      <c r="D27" t="s">
+        <v>57</v>
+      </c>
       <c r="G27" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="H27" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="B28" s="1">
+        <v>42942</v>
+      </c>
+      <c r="C28" s="1">
+        <v>41779</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
       <c r="G28" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="H28" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="B29" s="1">
+        <v>42942</v>
+      </c>
+      <c r="C29" s="1">
+        <v>41856</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
       <c r="G29" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="H29" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="B30" s="1">
+        <v>42942</v>
+      </c>
+      <c r="C30" s="1">
+        <v>41608</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
       <c r="G30" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="H30" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
+      <c r="B31" s="1">
+        <v>42942</v>
+      </c>
+      <c r="C31" s="2">
+        <v>41552</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
       <c r="G31" s="3" t="s">
         <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>44</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="1">
+        <v>42942</v>
+      </c>
+      <c r="C32" s="2">
+        <v>40966</v>
+      </c>
+      <c r="D32" t="s">
+        <v>57</v>
+      </c>
       <c r="G32" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
+      <c r="B33" s="1">
+        <v>42942</v>
+      </c>
+      <c r="C33" s="2">
+        <v>41191</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
       <c r="G33" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>46</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
+      <c r="B34" s="2">
+        <v>42944</v>
+      </c>
+      <c r="C34" s="2">
+        <v>41307</v>
+      </c>
+      <c r="D34" t="s">
+        <v>57</v>
+      </c>
       <c r="G34" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H34" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
+      <c r="B35" s="2">
+        <v>42944</v>
+      </c>
+      <c r="C35" s="2">
+        <v>40928</v>
+      </c>
+      <c r="D35" t="s">
+        <v>57</v>
+      </c>
       <c r="G35" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="B36" s="2">
+        <v>42944</v>
+      </c>
+      <c r="C36" s="2">
+        <v>40834</v>
+      </c>
+      <c r="D36" t="s">
+        <v>57</v>
+      </c>
       <c r="G36" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="H36" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1413,7 +1516,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1423,7 +1526,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -1433,7 +1536,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1443,7 +1546,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -1453,7 +1556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -1463,7 +1566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -1473,28 +1576,28 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="G44" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>

</xml_diff>

<commit_message>
updated et processing code
</commit_message>
<xml_diff>
--- a/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
+++ b/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Experiments/KM_SPEED_ACC/bing_data/speed_acc_child_gaze/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6120" yWindow="1320" windowWidth="25100" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="700" yWindow="1060" windowWidth="24860" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="68">
   <si>
     <t>subid</t>
   </si>
@@ -225,6 +220,12 @@
   </si>
   <si>
     <t xml:space="preserve">played with headphones during a couple of trials, and stood up for a couple of trials, but majority of session went well </t>
+  </si>
+  <si>
+    <t>exclude</t>
+  </si>
+  <si>
+    <t>keep</t>
   </si>
 </sst>
 </file>
@@ -278,11 +279,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="68">
+  <cellStyleXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -363,7 +366,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="68">
+  <cellStyles count="70">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -397,6 +400,7 @@
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -430,6 +434,7 @@
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
@@ -765,19 +770,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H54"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32:I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="8" max="8" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="12.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -802,8 +807,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="12.75" customHeight="1">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -822,8 +830,11 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -842,8 +853,11 @@
       <c r="H3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -862,8 +876,11 @@
       <c r="H4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -882,8 +899,11 @@
       <c r="H5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -905,8 +925,11 @@
       <c r="H6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -925,8 +948,11 @@
       <c r="H7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -945,8 +971,11 @@
       <c r="H8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="12.75" customHeight="1">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -965,8 +994,11 @@
       <c r="H9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="12.75" customHeight="1">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -985,8 +1017,11 @@
       <c r="H10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="12.75" customHeight="1">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1005,8 +1040,11 @@
       <c r="H11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="12.75" customHeight="1">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1025,8 +1063,11 @@
       <c r="H12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" customHeight="1">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1045,8 +1086,11 @@
       <c r="H13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="12.75" customHeight="1">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1065,8 +1109,11 @@
       <c r="H14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" customHeight="1">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1085,8 +1132,11 @@
       <c r="H15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" customHeight="1">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1105,8 +1155,11 @@
       <c r="H16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="12.75" customHeight="1">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1125,8 +1178,11 @@
       <c r="H17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" customHeight="1">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1145,8 +1201,11 @@
       <c r="H18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" customHeight="1">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1165,8 +1224,11 @@
       <c r="H19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" customHeight="1">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1185,8 +1247,11 @@
       <c r="H20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" customHeight="1">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1205,8 +1270,11 @@
       <c r="H21" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" customHeight="1">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1225,8 +1293,11 @@
       <c r="H22" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="12.75" customHeight="1">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1245,8 +1316,11 @@
       <c r="H23" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1265,8 +1339,11 @@
       <c r="H24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="12.75" customHeight="1">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -1285,8 +1362,11 @@
       <c r="H25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="12.75" customHeight="1">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1305,8 +1385,11 @@
       <c r="H26" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="12.75" customHeight="1">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1325,8 +1408,11 @@
       <c r="H27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="12.75" customHeight="1">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1345,8 +1431,11 @@
       <c r="H28" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="12.75" customHeight="1">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1365,8 +1454,11 @@
       <c r="H29" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="12.75" customHeight="1">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1385,8 +1477,11 @@
       <c r="H30" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="12.75" customHeight="1">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1405,8 +1500,11 @@
       <c r="H31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I31" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="12.75" customHeight="1">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1425,8 +1523,11 @@
       <c r="H32" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="12.75" customHeight="1">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -1445,8 +1546,11 @@
       <c r="H33" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="12.75" customHeight="1">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -1465,8 +1569,11 @@
       <c r="H34" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="12.75" customHeight="1">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -1485,8 +1592,11 @@
       <c r="H35" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="12.75" customHeight="1">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1505,8 +1615,11 @@
       <c r="H36" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="12.75" customHeight="1">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1516,7 +1629,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:9" ht="12.75" customHeight="1">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1526,7 +1639,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:9" ht="12.75" customHeight="1">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -1536,7 +1649,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:9" ht="12.75" customHeight="1">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1546,7 +1659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:9" ht="12.75" customHeight="1">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -1556,7 +1669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:9" ht="12.75" customHeight="1">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -1566,7 +1679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:9" ht="12.75" customHeight="1">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -1576,52 +1689,52 @@
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:9" ht="12.75" customHeight="1">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="G44" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:9" ht="12.75" customHeight="1">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:9" ht="12.75" customHeight="1">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="G46" s="3"/>
     </row>
-    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:9" ht="12.75" customHeight="1">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:9" ht="12.75" customHeight="1">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:3" ht="12.75" customHeight="1">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:3" ht="12.75" customHeight="1">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:3" ht="12.75" customHeight="1">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:3" ht="12.75" customHeight="1">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:3" ht="12.75" customHeight="1">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="2:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:3" ht="12.75" customHeight="1">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
@@ -1629,5 +1742,10 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated runsheets to add exclusions
</commit_message>
<xml_diff>
--- a/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
+++ b/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="1060" windowWidth="24860" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25100" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$2:$I$36</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -225,7 +228,7 @@
     <t>exclude</t>
   </si>
   <si>
-    <t>keep</t>
+    <t>include</t>
   </si>
 </sst>
 </file>
@@ -773,7 +776,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32:I36"/>
+      <selection activeCell="I2" sqref="I2:I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1739,6 +1742,7 @@
       <c r="C54" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="I2:I36"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
adding new et data
</commit_message>
<xml_diff>
--- a/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
+++ b/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
@@ -1,31 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Experiments/KM_SPEED_ACC/bing_data/speed_acc_child_gaze/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25100" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="25100" windowHeight="14680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$I$2:$I$36</definedName>
-  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="92">
   <si>
     <t>subid</t>
   </si>
@@ -225,10 +224,82 @@
     <t xml:space="preserve">played with headphones during a couple of trials, and stood up for a couple of trials, but majority of session went well </t>
   </si>
   <si>
-    <t>exclude</t>
-  </si>
-  <si>
-    <t>include</t>
+    <t xml:space="preserve">took off headphones during the last couple of sessions, but resumed and majority of session went well </t>
+  </si>
+  <si>
+    <t>did not want to wear headphones, couldn't calibrate</t>
+  </si>
+  <si>
+    <t>went well!</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_43</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_44</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_45</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_46</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_47</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_48</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_49</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_50</t>
+  </si>
+  <si>
+    <t>would not wear headphones</t>
+  </si>
+  <si>
+    <t>went well but he was pretending to be a dinosaur so he covered his eyes for a little while</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_51</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_52</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_53</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_54</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_55</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_56</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_57</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_58</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_59</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_60</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_61</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_62</t>
+  </si>
+  <si>
+    <t>SPEED_ACC_CHILD_GAZE_63</t>
   </si>
 </sst>
 </file>
@@ -282,13 +353,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="70">
+  <cellStyleXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -369,7 +438,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="70">
+  <cellStyles count="68">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -403,7 +472,6 @@
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -437,7 +505,6 @@
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
@@ -773,19 +840,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I54"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I36"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="8" max="8" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="12.75" customHeight="1">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -810,11 +877,8 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -833,11 +897,8 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -856,11 +917,8 @@
       <c r="H3" t="s">
         <v>58</v>
       </c>
-      <c r="I3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -879,11 +937,8 @@
       <c r="H4" t="s">
         <v>59</v>
       </c>
-      <c r="I4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -902,11 +957,8 @@
       <c r="H5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -928,11 +980,8 @@
       <c r="H6" t="s">
         <v>60</v>
       </c>
-      <c r="I6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -951,11 +1000,8 @@
       <c r="H7" t="s">
         <v>13</v>
       </c>
-      <c r="I7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -974,11 +1020,8 @@
       <c r="H8" t="s">
         <v>61</v>
       </c>
-      <c r="I8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -997,11 +1040,8 @@
       <c r="H9" t="s">
         <v>13</v>
       </c>
-      <c r="I9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1020,11 +1060,8 @@
       <c r="H10" t="s">
         <v>13</v>
       </c>
-      <c r="I10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1043,11 +1080,8 @@
       <c r="H11" t="s">
         <v>62</v>
       </c>
-      <c r="I11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1066,11 +1100,8 @@
       <c r="H12" t="s">
         <v>61</v>
       </c>
-      <c r="I12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1089,11 +1120,8 @@
       <c r="H13" t="s">
         <v>13</v>
       </c>
-      <c r="I13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1112,11 +1140,8 @@
       <c r="H14" t="s">
         <v>13</v>
       </c>
-      <c r="I14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1135,11 +1160,8 @@
       <c r="H15" t="s">
         <v>13</v>
       </c>
-      <c r="I15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1158,11 +1180,8 @@
       <c r="H16" t="s">
         <v>13</v>
       </c>
-      <c r="I16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1181,11 +1200,8 @@
       <c r="H17" t="s">
         <v>13</v>
       </c>
-      <c r="I17" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1204,11 +1220,8 @@
       <c r="H18" t="s">
         <v>13</v>
       </c>
-      <c r="I18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1227,11 +1240,8 @@
       <c r="H19" t="s">
         <v>63</v>
       </c>
-      <c r="I19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1250,11 +1260,8 @@
       <c r="H20" t="s">
         <v>13</v>
       </c>
-      <c r="I20" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1273,11 +1280,8 @@
       <c r="H21" t="s">
         <v>61</v>
       </c>
-      <c r="I21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1296,11 +1300,8 @@
       <c r="H22" t="s">
         <v>64</v>
       </c>
-      <c r="I22" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1319,11 +1320,8 @@
       <c r="H23" t="s">
         <v>61</v>
       </c>
-      <c r="I23" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1342,11 +1340,8 @@
       <c r="H24" t="s">
         <v>13</v>
       </c>
-      <c r="I24" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -1365,11 +1360,8 @@
       <c r="H25" t="s">
         <v>13</v>
       </c>
-      <c r="I25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1388,11 +1380,8 @@
       <c r="H26" t="s">
         <v>13</v>
       </c>
-      <c r="I26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1411,11 +1400,8 @@
       <c r="H27" t="s">
         <v>13</v>
       </c>
-      <c r="I27" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1434,11 +1420,8 @@
       <c r="H28" t="s">
         <v>13</v>
       </c>
-      <c r="I28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1457,11 +1440,8 @@
       <c r="H29" t="s">
         <v>13</v>
       </c>
-      <c r="I29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1480,11 +1460,8 @@
       <c r="H30" t="s">
         <v>65</v>
       </c>
-      <c r="I30" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1503,11 +1480,8 @@
       <c r="H31" t="s">
         <v>61</v>
       </c>
-      <c r="I31" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1526,11 +1500,8 @@
       <c r="H32" t="s">
         <v>13</v>
       </c>
-      <c r="I32" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -1549,11 +1520,8 @@
       <c r="H33" t="s">
         <v>13</v>
       </c>
-      <c r="I33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -1572,11 +1540,8 @@
       <c r="H34" t="s">
         <v>13</v>
       </c>
-      <c r="I34" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -1595,11 +1560,8 @@
       <c r="H35" t="s">
         <v>13</v>
       </c>
-      <c r="I35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1618,138 +1580,356 @@
       <c r="H36" t="s">
         <v>13</v>
       </c>
-      <c r="I36" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="B37" s="2">
+        <v>42949</v>
+      </c>
+      <c r="C37" s="2">
+        <v>41672</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
       <c r="G37" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="12.75" customHeight="1">
+      <c r="H37" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>50</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="B38" s="2">
+        <v>42949</v>
+      </c>
+      <c r="C38" s="2">
+        <v>41007</v>
+      </c>
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
       <c r="G38" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="12.75" customHeight="1">
+      <c r="H38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="B39" s="2">
+        <v>42949</v>
+      </c>
+      <c r="C39" s="2">
+        <v>41016</v>
+      </c>
+      <c r="D39" t="s">
+        <v>12</v>
+      </c>
       <c r="G39" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="12.75" customHeight="1">
+      <c r="H39" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
+      <c r="B40" s="2">
+        <v>42951</v>
+      </c>
+      <c r="C40" s="2">
+        <v>41388</v>
+      </c>
+      <c r="D40" t="s">
+        <v>12</v>
+      </c>
       <c r="G40" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="12.75" customHeight="1">
+      <c r="H40" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>53</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="2">
+        <v>42965</v>
+      </c>
       <c r="C41" s="2"/>
+      <c r="D41" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
       <c r="G41" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="12.75" customHeight="1">
+      <c r="H41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>54</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="2">
+        <v>42965</v>
+      </c>
       <c r="C42" s="2"/>
+      <c r="D42" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
       <c r="G42" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="12.75" customHeight="1">
+      <c r="H42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>55</v>
       </c>
-      <c r="B43" s="2"/>
+      <c r="B43" s="2">
+        <v>42965</v>
+      </c>
       <c r="C43" s="2"/>
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
       <c r="G43" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="12.75" customHeight="1">
-      <c r="B44" s="2"/>
+      <c r="H43" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="2">
+        <v>42965</v>
+      </c>
       <c r="C44" s="2"/>
+      <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
       <c r="G44" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="12.75" customHeight="1">
-      <c r="B45" s="2"/>
+      <c r="H44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="2">
+        <v>42969</v>
+      </c>
       <c r="C45" s="2"/>
-      <c r="G45" s="3"/>
-    </row>
-    <row r="46" spans="1:9" ht="12.75" customHeight="1">
+      <c r="G45" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>71</v>
+      </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="G46" s="3"/>
-    </row>
-    <row r="47" spans="1:9" ht="12.75" customHeight="1">
+      <c r="G46" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>72</v>
+      </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-    </row>
-    <row r="48" spans="1:9" ht="12.75" customHeight="1">
+      <c r="G47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
+        <v>74</v>
+      </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>75</v>
+      </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
+        <v>76</v>
+      </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
+        <v>79</v>
+      </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
+        <v>80</v>
+      </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
-    </row>
-    <row r="54" spans="2:3" ht="12.75" customHeight="1">
+      <c r="G53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>81</v>
+      </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
+      <c r="G54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
+        <v>82</v>
+      </c>
+      <c r="G55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" t="s">
+        <v>83</v>
+      </c>
+      <c r="G56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
+        <v>84</v>
+      </c>
+      <c r="G57" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>85</v>
+      </c>
+      <c r="G58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>86</v>
+      </c>
+      <c r="G59" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>87</v>
+      </c>
+      <c r="G60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>88</v>
+      </c>
+      <c r="G61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>89</v>
+      </c>
+      <c r="G62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>90</v>
+      </c>
+      <c r="G63" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" t="s">
+        <v>91</v>
+      </c>
+      <c r="G64" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="I2:I36"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new noise and gaze kid data
</commit_message>
<xml_diff>
--- a/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
+++ b/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="94">
   <si>
     <t>subid</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t>SPEED_ACC_CHILD_GAZE_63</t>
+  </si>
+  <si>
+    <t>stopped early; also may have already played this game with tami</t>
+  </si>
+  <si>
+    <t>mom and sister in the room so he was distracted</t>
   </si>
 </sst>
 </file>
@@ -842,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1753,38 +1759,80 @@
         <v>42969</v>
       </c>
       <c r="C45" s="2"/>
+      <c r="D45" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
       <c r="G45" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="H45" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="2"/>
+      <c r="B46" s="2">
+        <v>42969</v>
+      </c>
       <c r="C46" s="2"/>
+      <c r="D46" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
       <c r="G46" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="H46" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="2"/>
+      <c r="B47" s="2">
+        <v>42970</v>
+      </c>
       <c r="C47" s="2"/>
+      <c r="D47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E47">
+        <v>5</v>
+      </c>
       <c r="G47" t="s">
         <v>10</v>
+      </c>
+      <c r="H47" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="2"/>
+      <c r="B48" s="2">
+        <v>42970</v>
+      </c>
       <c r="C48" s="2"/>
+      <c r="D48" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
       <c r="G48" t="s">
         <v>10</v>
+      </c>
+      <c r="H48" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
streamlined and parallelized et processing code across expts
</commit_message>
<xml_diff>
--- a/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
+++ b/data/0a_demographics/speed_acc_child_gaze_Runsheet_Bing.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Experiments/KM_SPEED_ACC/bing_data/speed_acc_child_gaze/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="25100" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25100" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="97">
   <si>
     <t>subid</t>
   </si>
@@ -306,6 +301,15 @@
   </si>
   <si>
     <t>mom and sister in the room so he was distracted</t>
+  </si>
+  <si>
+    <t>keep_runsheet</t>
+  </si>
+  <si>
+    <t>keep</t>
+  </si>
+  <si>
+    <t>exclude</t>
   </si>
 </sst>
 </file>
@@ -359,11 +363,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="68">
+  <cellStyleXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -444,7 +450,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="68">
+  <cellStyles count="70">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -478,6 +484,7 @@
     <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -511,6 +518,7 @@
     <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
@@ -846,19 +854,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41:F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="8" max="8" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" ht="12.75" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -883,8 +891,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="12.75" customHeight="1">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -903,8 +914,11 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" customHeight="1">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -923,8 +937,11 @@
       <c r="H3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" customHeight="1">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -943,8 +960,11 @@
       <c r="H4" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="12.75" customHeight="1">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -963,8 +983,11 @@
       <c r="H5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" customHeight="1">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -986,8 +1009,11 @@
       <c r="H6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="12.75" customHeight="1">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1006,8 +1032,11 @@
       <c r="H7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" customHeight="1">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -1026,8 +1055,11 @@
       <c r="H8" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="12.75" customHeight="1">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1046,8 +1078,11 @@
       <c r="H9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="12.75" customHeight="1">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1066,8 +1101,11 @@
       <c r="H10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="12.75" customHeight="1">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1086,8 +1124,11 @@
       <c r="H11" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="12.75" customHeight="1">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1106,8 +1147,11 @@
       <c r="H12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" customHeight="1">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1126,8 +1170,11 @@
       <c r="H13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="12.75" customHeight="1">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1146,8 +1193,11 @@
       <c r="H14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" customHeight="1">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -1166,8 +1216,11 @@
       <c r="H15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" customHeight="1">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1186,8 +1239,11 @@
       <c r="H16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="12.75" customHeight="1">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -1206,8 +1262,11 @@
       <c r="H17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="12.75" customHeight="1">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -1226,8 +1285,11 @@
       <c r="H18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="12.75" customHeight="1">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1246,8 +1308,11 @@
       <c r="H19" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="12.75" customHeight="1">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1266,8 +1331,11 @@
       <c r="H20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="12.75" customHeight="1">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1286,8 +1354,11 @@
       <c r="H21" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I21" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12.75" customHeight="1">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -1306,8 +1377,11 @@
       <c r="H22" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I22" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="12.75" customHeight="1">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -1326,8 +1400,11 @@
       <c r="H23" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="12.75" customHeight="1">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1346,8 +1423,11 @@
       <c r="H24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="12.75" customHeight="1">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -1366,8 +1446,11 @@
       <c r="H25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I25" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="12.75" customHeight="1">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1386,8 +1469,11 @@
       <c r="H26" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="12.75" customHeight="1">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1406,8 +1492,11 @@
       <c r="H27" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="12.75" customHeight="1">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1426,8 +1515,11 @@
       <c r="H28" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="12.75" customHeight="1">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1446,8 +1538,11 @@
       <c r="H29" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="12.75" customHeight="1">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1466,8 +1561,11 @@
       <c r="H30" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I30" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="12.75" customHeight="1">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1486,8 +1584,11 @@
       <c r="H31" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="12.75" customHeight="1">
       <c r="A32" t="s">
         <v>44</v>
       </c>
@@ -1506,8 +1607,11 @@
       <c r="H32" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="12.75" customHeight="1">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -1526,8 +1630,11 @@
       <c r="H33" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="12.75" customHeight="1">
       <c r="A34" t="s">
         <v>46</v>
       </c>
@@ -1546,8 +1653,11 @@
       <c r="H34" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="12.75" customHeight="1">
       <c r="A35" t="s">
         <v>47</v>
       </c>
@@ -1566,8 +1676,11 @@
       <c r="H35" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I35" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="12.75" customHeight="1">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -1586,8 +1699,11 @@
       <c r="H36" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="12.75" customHeight="1">
       <c r="A37" t="s">
         <v>49</v>
       </c>
@@ -1606,8 +1722,11 @@
       <c r="H37" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="12.75" customHeight="1">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1626,8 +1745,11 @@
       <c r="H38" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="12.75" customHeight="1">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -1646,8 +1768,11 @@
       <c r="H39" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="12.75" customHeight="1">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -1666,8 +1791,11 @@
       <c r="H40" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="12.75" customHeight="1">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -1678,7 +1806,7 @@
       <c r="D41" t="s">
         <v>12</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>3</v>
       </c>
       <c r="G41" s="3" t="s">
@@ -1687,8 +1815,11 @@
       <c r="H41" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I41" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="12.75" customHeight="1">
       <c r="A42" t="s">
         <v>54</v>
       </c>
@@ -1699,7 +1830,7 @@
       <c r="D42" t="s">
         <v>12</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>4</v>
       </c>
       <c r="G42" s="3" t="s">
@@ -1708,8 +1839,11 @@
       <c r="H42" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="12.75" customHeight="1">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -1720,7 +1854,7 @@
       <c r="D43" t="s">
         <v>12</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>3</v>
       </c>
       <c r="G43" s="3" t="s">
@@ -1729,8 +1863,11 @@
       <c r="H43" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="12.75" customHeight="1">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -1741,7 +1878,7 @@
       <c r="D44" t="s">
         <v>12</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>3</v>
       </c>
       <c r="G44" s="3" t="s">
@@ -1750,8 +1887,11 @@
       <c r="H44" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="12.75" customHeight="1">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -1762,7 +1902,7 @@
       <c r="D45" t="s">
         <v>57</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>4</v>
       </c>
       <c r="G45" s="3" t="s">
@@ -1771,8 +1911,11 @@
       <c r="H45" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="12.75" customHeight="1">
       <c r="A46" t="s">
         <v>71</v>
       </c>
@@ -1783,7 +1926,7 @@
       <c r="D46" t="s">
         <v>57</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>3</v>
       </c>
       <c r="G46" s="3" t="s">
@@ -1792,8 +1935,11 @@
       <c r="H46" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I46" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="12.75" customHeight="1">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -1804,7 +1950,7 @@
       <c r="D47" t="s">
         <v>12</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>5</v>
       </c>
       <c r="G47" t="s">
@@ -1813,8 +1959,11 @@
       <c r="H47" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I47" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="12.75" customHeight="1">
       <c r="A48" t="s">
         <v>73</v>
       </c>
@@ -1825,7 +1974,7 @@
       <c r="D48" t="s">
         <v>12</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>4</v>
       </c>
       <c r="G48" t="s">
@@ -1834,8 +1983,11 @@
       <c r="H48" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="12.75" customHeight="1">
       <c r="A49" t="s">
         <v>74</v>
       </c>
@@ -1845,7 +1997,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:7" ht="12.75" customHeight="1">
       <c r="A50" t="s">
         <v>75</v>
       </c>
@@ -1855,7 +2007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:7" ht="12.75" customHeight="1">
       <c r="A51" t="s">
         <v>76</v>
       </c>
@@ -1865,7 +2017,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:7" ht="12.75" customHeight="1">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -1875,7 +2027,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:7" ht="12.75" customHeight="1">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -1885,7 +2037,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:7" ht="12.75" customHeight="1">
       <c r="A54" t="s">
         <v>81</v>
       </c>
@@ -1895,7 +2047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:7" ht="12.75" customHeight="1">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -1903,7 +2055,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:7" ht="12.75" customHeight="1">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -1911,7 +2063,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:7" ht="12.75" customHeight="1">
       <c r="A57" t="s">
         <v>84</v>
       </c>
@@ -1919,7 +2071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:7" ht="12.75" customHeight="1">
       <c r="A58" t="s">
         <v>85</v>
       </c>
@@ -1927,7 +2079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:7" ht="12.75" customHeight="1">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -1935,7 +2087,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:7" ht="12.75" customHeight="1">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -1943,7 +2095,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:7" ht="12.75" customHeight="1">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -1951,7 +2103,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:7" ht="12.75" customHeight="1">
       <c r="A62" t="s">
         <v>89</v>
       </c>
@@ -1959,7 +2111,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:7" ht="12.75" customHeight="1">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -1967,7 +2119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:7" ht="12.75" customHeight="1">
       <c r="A64" t="s">
         <v>91</v>
       </c>
@@ -1979,5 +2131,10 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>